<commit_message>
Script updates and files created
</commit_message>
<xml_diff>
--- a/RAP/Scoring Metadata/RAP_Metadata.xlsx
+++ b/RAP/Scoring Metadata/RAP_Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/mcneelys_si_edu/Documents/Desktop/GitHub/Oysters/RAP/Scoring Metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{DACE2786-0239-4288-B2DE-44AD3C1C6C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02700A52-58E6-43CD-BD55-1B1AB217918B}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{DACE2786-0239-4288-B2DE-44AD3C1C6C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27ED6F15-B588-442E-B959-9D761C393105}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{EC35DC18-0F9C-487E-B5FA-180721239FD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>MM/DD/YYYY</t>
   </si>
@@ -105,6 +105,30 @@
   </si>
   <si>
     <t>Site longitude.</t>
+  </si>
+  <si>
+    <t>Max_Habscore</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Difference +2') Difference between Habscore_a and Habscore_b is &gt;=2; score difference is worth double checking.</t>
+  </si>
+  <si>
+    <t>NA) Difference between Habscore_a and Habscore_b is &lt;2; score difference is not notable.</t>
+  </si>
+  <si>
+    <t>Check_Warnings</t>
+  </si>
+  <si>
+    <t>NA) Warning column did not produce a warning that recommends a second look.</t>
+  </si>
+  <si>
+    <t>Good') Warning was double checked for the site and the scores were appropriately assigned.</t>
+  </si>
+  <si>
+    <t>REVISIT') Warning was double checked for the site and the scores were NOT appropriately assigned.</t>
   </si>
 </sst>
 </file>
@@ -148,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,6 +182,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3708EAC0-DACD-4342-9DAE-E0297093C888}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -489,9 +516,12 @@
     <col min="6" max="6" width="30.6328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="37.453125" style="2" customWidth="1"/>
     <col min="8" max="8" width="22" style="2" customWidth="1"/>
+    <col min="9" max="9" width="37.6328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="34.81640625" customWidth="1"/>
+    <col min="11" max="11" width="35.08984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -516,8 +546,17 @@
       <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -542,37 +581,73 @@
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="G6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>